<commit_message>
Updated ReadME with the tutorial from youtube
</commit_message>
<xml_diff>
--- a/Configuration_template.xlsx
+++ b/Configuration_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhil.kondabala\Documents\GitHub\CFARS_datawrangling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhil.kondabala\Documents\GitHub\CFARS_SS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{20C921D8-4EFF-4F24-B1CE-64A2F39EC99F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DE11C7C6-3F52-4348-9228-64C7C190D15A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13305" xr2:uid="{A269487F-E818-43E3-8C7E-ED7B59939733}"/>
   </bookViews>
@@ -481,7 +481,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +618,7 @@
           <x14:formula1>
             <xm:f>Lable!$A$1:$A$28</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B39</xm:sqref>
+          <xm:sqref>B33:B39 B2:B32</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -630,9 +630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -653,50 +651,53 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:A12">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
got the dataframes organized in the original format.
</commit_message>
<xml_diff>
--- a/Configuration_template.xlsx
+++ b/Configuration_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhil.kondabala\Documents\GitHub\CFARS_SS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DE11C7C6-3F52-4348-9228-64C7C190D15A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C4ED09AF-DCE3-4961-ADDF-F81553FBE3AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13305" xr2:uid="{A269487F-E818-43E3-8C7E-ED7B59939733}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Date and Time</t>
   </si>
@@ -116,6 +116,27 @@
   </si>
   <si>
     <t>corrTI_RSD_WS</t>
+  </si>
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
+  <si>
+    <t>filter1</t>
+  </si>
+  <si>
+    <t>filter2</t>
+  </si>
+  <si>
+    <t>60m Wind Speed CorrWS</t>
+  </si>
+  <si>
+    <t>60m Wind Turbulence CorrWS</t>
+  </si>
+  <si>
+    <t>60m Wind Speed Corr TI</t>
+  </si>
+  <si>
+    <t>60m Wind Turbulence CorrTI</t>
   </si>
 </sst>
 </file>
@@ -478,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F08FE4-0760-457A-AC2E-B11E8BB556DD}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,110 +521,157 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>